<commit_message>
Created tests and utils for the test
</commit_message>
<xml_diff>
--- a/src/test/resources/correctCertificate.xlsx
+++ b/src/test/resources/correctCertificate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB95BE8F-8FE6-4622-90DF-812EE605BBAC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5032E08-CB2E-49F8-A64D-604A1DC9A77B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="15">
   <si>
     <t>Course 1</t>
   </si>
@@ -49,19 +49,22 @@
     <t>Course 5</t>
   </si>
   <si>
-    <t>PR</t>
-  </si>
-  <si>
     <t>Course 6</t>
   </si>
   <si>
     <t>VO</t>
   </si>
   <si>
-    <t>SE</t>
-  </si>
-  <si>
-    <t>UE</t>
+    <t>Course 7</t>
+  </si>
+  <si>
+    <t>Course 8</t>
+  </si>
+  <si>
+    <t>Course 9</t>
+  </si>
+  <si>
+    <t>Course 10</t>
   </si>
 </sst>
 </file>
@@ -380,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:I9"/>
+  <dimension ref="A4:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -393,7 +396,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -422,7 +425,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -451,7 +454,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -509,7 +512,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -535,10 +538,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
@@ -559,6 +562,122 @@
         <v>43471</v>
       </c>
       <c r="I9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>43471</v>
+      </c>
+      <c r="I10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>43471</v>
+      </c>
+      <c r="I11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>43471</v>
+      </c>
+      <c r="I12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>43471</v>
+      </c>
+      <c r="I13" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>